<commit_message>
Added some logic to scoring model to avoid mistakes when the form is filled out
</commit_message>
<xml_diff>
--- a/Score Model and AHP/Gewichtung%20Nutzwertanalyse%20V3.xlsx
+++ b/Score Model and AHP/Gewichtung%20Nutzwertanalyse%20V3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium\Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicklas\WebstormProjects\Block\Score Model and AHP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -218,7 +218,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -356,6 +356,12 @@
       <sz val="11"/>
       <color indexed="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF363636"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -792,18 +798,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -819,11 +816,30 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1147,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1169,720 +1185,1008 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="1"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19">
         <v>1</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="19">
         <v>2</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="19">
         <v>3</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="19">
         <v>4</v>
       </c>
-      <c r="H5" s="5"/>
+      <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5" t="s">
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18">
         <v>1</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="D7" s="18"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="21">
+        <f>COUNTIF(D7:G7,1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18">
         <v>2</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="D8" s="17">
+        <f>E7</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="21">
+        <f>COUNTIF(D8:G8,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="18">
         <v>3</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="D9" s="17">
+        <f>F7</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="17">
+        <f>F8</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="18"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="21">
+        <f>COUNTIF(D9:G9,3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18">
         <v>4</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="18"/>
+      <c r="C10" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="1"/>
+      <c r="D10" s="17">
+        <f>G7</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="17">
+        <f>G8</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="17">
+        <f>G9</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="18"/>
+      <c r="H10" s="21">
+        <f>COUNTIF(D10:G10,4)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="11"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="8"/>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19">
         <v>1</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="19">
         <v>2</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="19">
         <v>3</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="19">
         <v>4</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="19">
         <v>5</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="19">
         <v>6</v>
       </c>
-      <c r="J13" s="12"/>
+      <c r="J13" s="18"/>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5" t="s">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="J14" s="18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="18">
         <v>1</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5" t="s">
+      <c r="B15" s="18"/>
+      <c r="C15" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="D15" s="18"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="21">
+        <f>COUNTIF(D15:I15,1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18">
         <v>2</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="D16" s="17">
+        <f>E15</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="18"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="21">
+        <f>COUNTIF(D16:I16,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="18">
         <v>3</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="D17" s="17">
+        <f>F15</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="17">
+        <f>F16</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="18"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="21">
+        <f>COUNTIF(D17:I17,3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="18">
         <v>4</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="D18" s="17">
+        <f>G15</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="17">
+        <f>G16</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="17">
+        <f>G17</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="18"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="21">
+        <f>COUNTIF(D18:I18,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="18">
         <v>5</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+      <c r="D19" s="17">
+        <f>H15</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="17">
+        <f>H16</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="17">
+        <f>H17</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="17">
+        <f>H18</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="18"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="21">
+        <f>COUNTIF(D19:I19,5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="18">
         <v>6</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5" t="s">
+      <c r="B20" s="18"/>
+      <c r="C20" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="1"/>
+      <c r="D20" s="17">
+        <f>I15</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="17">
+        <f>I16</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="17">
+        <f>I17</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="17">
+        <f>I18</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="17">
+        <f>I19</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="18"/>
+      <c r="J20" s="21">
+        <f>COUNTIF(D20:I20,6)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="2" t="s">
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="1"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="17"/>
     </row>
     <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6">
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19">
         <v>1</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="19">
         <v>2</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="19">
         <v>3</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="19">
         <v>4</v>
       </c>
-      <c r="H25" s="5"/>
+      <c r="H25" s="18"/>
     </row>
     <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5" t="s">
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G26" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="H26" s="18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+    <row r="27" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="18">
         <v>1</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="D27" s="18"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="21">
+        <f>COUNTIF(D27:G27,1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="18">
         <v>2</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+      <c r="D28" s="17">
+        <f>E27</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="18"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="21">
+        <f>COUNTIF(D28:G28,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="18">
         <v>3</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+      <c r="D29" s="17">
+        <f>F27</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="17">
+        <f>F28</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="18"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="21">
+        <f>COUNTIF(D29:G29,3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="18">
         <v>4</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5" t="s">
+      <c r="B30" s="18"/>
+      <c r="C30" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="1"/>
+      <c r="D30" s="17">
+        <f>G27</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="17">
+        <f>G28</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="17">
+        <f>G29</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="18"/>
+      <c r="H30" s="21">
+        <f>COUNTIF(D30:G30,4)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="16"/>
-      <c r="O35" s="15"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="11"/>
     </row>
     <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13">
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10">
         <v>1</v>
       </c>
-      <c r="E36" s="13">
+      <c r="E36" s="10">
         <v>2</v>
       </c>
-      <c r="F36" s="13">
+      <c r="F36" s="10">
         <v>3</v>
       </c>
-      <c r="G36" s="13">
+      <c r="G36" s="10">
         <v>4</v>
       </c>
-      <c r="H36" s="13">
+      <c r="H36" s="10">
         <v>5</v>
       </c>
-      <c r="I36" s="13">
+      <c r="I36" s="10">
         <v>6</v>
       </c>
-      <c r="J36" s="13">
+      <c r="J36" s="10">
         <v>7</v>
       </c>
-      <c r="K36" s="13">
+      <c r="K36" s="10">
         <v>8</v>
       </c>
-      <c r="L36" s="13">
+      <c r="L36" s="10">
         <v>9</v>
       </c>
-      <c r="M36" s="13">
+      <c r="M36" s="10">
         <v>10</v>
       </c>
-      <c r="N36" s="13"/>
+      <c r="N36" s="10"/>
     </row>
     <row r="37" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5" t="s">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F37" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="G37" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="H37" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I37" s="8" t="s">
+      <c r="I37" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J37" s="8" t="s">
+      <c r="J37" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K37" s="5" t="s">
+      <c r="K37" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L37" s="5" t="s">
+      <c r="L37" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="M37" s="5" t="s">
+      <c r="M37" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N37" s="5" t="s">
+      <c r="N37" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
+    <row r="38" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
         <v>1</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="5"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="1"/>
-    </row>
-    <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
+      <c r="D38" s="2"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="21">
+        <f>COUNTIF(D38:M38,1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
         <v>2</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="7"/>
-      <c r="M39" s="7"/>
-      <c r="N39" s="1"/>
-    </row>
-    <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
+      <c r="D39" s="17">
+        <f>E38</f>
+        <v>0</v>
+      </c>
+      <c r="E39" s="7"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="21">
+        <f>COUNTIF(D39:M39,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
         <v>3</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
-      <c r="L40" s="7"/>
-      <c r="M40" s="7"/>
-      <c r="N40" s="1"/>
-    </row>
-    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
+      <c r="D40" s="17">
+        <f>F38</f>
+        <v>0</v>
+      </c>
+      <c r="E40" s="17">
+        <f>F39</f>
+        <v>0</v>
+      </c>
+      <c r="F40" s="2"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="21">
+        <f>COUNTIF(D40:M40,3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
         <v>4</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="7"/>
-      <c r="N41" s="1"/>
-    </row>
-    <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
+      <c r="D41" s="17">
+        <f>G38</f>
+        <v>0</v>
+      </c>
+      <c r="E41" s="17">
+        <f>G39</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="17">
+        <f>G40</f>
+        <v>0</v>
+      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="21">
+        <f>COUNTIF(D41:M41,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
         <v>5</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="7"/>
-      <c r="N42" s="1"/>
-    </row>
-    <row r="43" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="5">
+      <c r="D42" s="17">
+        <f>H38</f>
+        <v>0</v>
+      </c>
+      <c r="E42" s="17">
+        <f>H39</f>
+        <v>0</v>
+      </c>
+      <c r="F42" s="17">
+        <f>H40</f>
+        <v>0</v>
+      </c>
+      <c r="G42" s="17">
+        <f>H41</f>
+        <v>0</v>
+      </c>
+      <c r="H42" s="2"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="21">
+        <f>COUNTIF(D42:M42,5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
         <v>6</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="7"/>
-      <c r="M43" s="7"/>
-      <c r="N43" s="1"/>
-    </row>
-    <row r="44" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="5">
+      <c r="D43" s="17">
+        <f>I38</f>
+        <v>0</v>
+      </c>
+      <c r="E43" s="17">
+        <f>I39</f>
+        <v>0</v>
+      </c>
+      <c r="F43" s="17">
+        <f>I40</f>
+        <v>0</v>
+      </c>
+      <c r="G43" s="17">
+        <f>I41</f>
+        <v>0</v>
+      </c>
+      <c r="H43" s="17">
+        <f>I42</f>
+        <v>0</v>
+      </c>
+      <c r="I43" s="2"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="21">
+        <f>COUNTIF(D43:M43,6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
         <v>7</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="7"/>
-      <c r="M44" s="7"/>
-      <c r="N44" s="1"/>
-    </row>
-    <row r="45" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="5">
+      <c r="D44" s="17">
+        <f>J38</f>
+        <v>0</v>
+      </c>
+      <c r="E44" s="17">
+        <f>J39</f>
+        <v>0</v>
+      </c>
+      <c r="F44" s="17">
+        <f>J40</f>
+        <v>0</v>
+      </c>
+      <c r="G44" s="17">
+        <f>J41</f>
+        <v>0</v>
+      </c>
+      <c r="H44" s="17">
+        <f>J42</f>
+        <v>0</v>
+      </c>
+      <c r="I44" s="17">
+        <f>J43</f>
+        <v>0</v>
+      </c>
+      <c r="J44" s="2"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="21">
+        <f>COUNTIF(D44:M44,7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
         <v>8</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="7"/>
-      <c r="M45" s="7"/>
-      <c r="N45" s="1"/>
-    </row>
-    <row r="46" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="5">
+      <c r="D45" s="17">
+        <f>K38</f>
+        <v>0</v>
+      </c>
+      <c r="E45" s="17">
+        <f>K39</f>
+        <v>0</v>
+      </c>
+      <c r="F45" s="17">
+        <f>K40</f>
+        <v>0</v>
+      </c>
+      <c r="G45" s="17">
+        <f>K41</f>
+        <v>0</v>
+      </c>
+      <c r="H45" s="17">
+        <f>K42</f>
+        <v>0</v>
+      </c>
+      <c r="I45" s="17">
+        <f>K43</f>
+        <v>0</v>
+      </c>
+      <c r="J45" s="17">
+        <f>K44</f>
+        <v>0</v>
+      </c>
+      <c r="K45" s="2"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="21">
+        <f>COUNTIF(D45:M45,8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
         <v>9</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="7"/>
-      <c r="N46" s="1"/>
-    </row>
-    <row r="47" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="5">
+      <c r="D46" s="17">
+        <f>L38</f>
+        <v>0</v>
+      </c>
+      <c r="E46" s="17">
+        <f>L39</f>
+        <v>0</v>
+      </c>
+      <c r="F46" s="17">
+        <f>L40</f>
+        <v>0</v>
+      </c>
+      <c r="G46" s="17">
+        <f>L41</f>
+        <v>0</v>
+      </c>
+      <c r="H46" s="17">
+        <f>L42</f>
+        <v>0</v>
+      </c>
+      <c r="I46" s="17">
+        <f>L43</f>
+        <v>0</v>
+      </c>
+      <c r="J46" s="17">
+        <f>L44</f>
+        <v>0</v>
+      </c>
+      <c r="K46" s="17">
+        <f>L45</f>
+        <v>0</v>
+      </c>
+      <c r="L46" s="2"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="21">
+        <f>COUNTIF(D46:M46,9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
         <v>10</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="1"/>
+      <c r="D47" s="17">
+        <f>M38</f>
+        <v>0</v>
+      </c>
+      <c r="E47" s="17">
+        <f>M39</f>
+        <v>0</v>
+      </c>
+      <c r="F47" s="17">
+        <f>M40</f>
+        <v>0</v>
+      </c>
+      <c r="G47" s="17">
+        <f>M41</f>
+        <v>0</v>
+      </c>
+      <c r="H47" s="17">
+        <f>M42</f>
+        <v>0</v>
+      </c>
+      <c r="I47" s="17">
+        <f>M43</f>
+        <v>0</v>
+      </c>
+      <c r="J47" s="17">
+        <f>M44</f>
+        <v>0</v>
+      </c>
+      <c r="K47" s="17">
+        <f>M45</f>
+        <v>0</v>
+      </c>
+      <c r="L47" s="17">
+        <f>M46</f>
+        <v>0</v>
+      </c>
+      <c r="M47" s="2"/>
+      <c r="N47" s="21">
+        <f>COUNTIF(D47:M47,10)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="9:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I54" t="s">
@@ -1897,7 +2201,7 @@
     <mergeCell ref="A12:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1950,84 +2254,84 @@
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="3"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15"/>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3">
         <v>1</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="3">
         <v>2</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="3">
         <v>3</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5" t="s">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+      <c r="A22" s="2">
         <v>1</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="7">
+      <c r="C22" s="2"/>
+      <c r="D22" s="4">
         <v>1</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="4">
         <v>1</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+      <c r="A23" s="2">
         <v>2</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="7">
+      <c r="D23" s="2"/>
+      <c r="E23" s="4">
         <v>2</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+      <c r="A24" s="2">
         <v>3</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="5"/>
+      <c r="E24" s="2"/>
       <c r="F24" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added WebVR API do display sensor values of oculus rift in console.
</commit_message>
<xml_diff>
--- a/Score Model and AHP/Gewichtung%20Nutzwertanalyse%20V3.xlsx
+++ b/Score Model and AHP/Gewichtung%20Nutzwertanalyse%20V3.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Gewichtung Kriterien" sheetId="1" r:id="rId1"/>
     <sheet name="Anleitung" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -217,7 +217,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -818,18 +818,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -839,6 +827,18 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -899,7 +899,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1185,143 +1185,143 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="17"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15">
         <v>1</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="15">
         <v>2</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="15">
         <v>3</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="15">
         <v>4</v>
       </c>
-      <c r="H5" s="18"/>
+      <c r="H5" s="14"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18">
+      <c r="A7" s="14">
         <v>1</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="21">
+      <c r="D7" s="14"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="17">
         <f>COUNTIF(D7:G7,1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18">
+      <c r="A8" s="14">
         <v>2</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="13">
         <f>E7</f>
         <v>0</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="21">
+      <c r="E8" s="14"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="17">
         <f>COUNTIF(D8:G8,2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18">
+      <c r="A9" s="14">
         <v>3</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="13">
         <f>F7</f>
         <v>0</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="13">
         <f>F8</f>
         <v>0</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="21">
+      <c r="F9" s="14"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17">
         <f>COUNTIF(D9:G9,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18">
+      <c r="A10" s="14">
         <v>4</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18" t="s">
+      <c r="B10" s="14"/>
+      <c r="C10" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="13">
         <f>G7</f>
         <v>0</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="13">
         <f>G8</f>
         <v>0</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="13">
         <f>G9</f>
         <v>0</v>
       </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="21">
+      <c r="G10" s="14"/>
+      <c r="H10" s="17">
         <f>COUNTIF(D10:G10,4)</f>
         <v>0</v>
       </c>
@@ -1337,395 +1337,395 @@
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
       <c r="K12" s="8"/>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15">
         <v>1</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="15">
         <v>2</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="15">
         <v>3</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="15">
         <v>4</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="15">
         <v>5</v>
       </c>
-      <c r="I13" s="19">
+      <c r="I13" s="15">
         <v>6</v>
       </c>
-      <c r="J13" s="18"/>
+      <c r="J13" s="14"/>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18" t="s">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="18" t="s">
+      <c r="I14" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="J14" s="18" t="s">
+      <c r="J14" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="18">
+      <c r="A15" s="14">
         <v>1</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18" t="s">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="21">
+      <c r="D15" s="14"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="17">
         <f>COUNTIF(D15:I15,1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="18">
+      <c r="A16" s="14">
         <v>2</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="13">
         <f>E15</f>
         <v>0</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="21">
+      <c r="E16" s="14"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="17">
         <f>COUNTIF(D16:I16,2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18">
+      <c r="A17" s="14">
         <v>3</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="13">
         <f>F15</f>
         <v>0</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="13">
         <f>F16</f>
         <v>0</v>
       </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="21">
+      <c r="F17" s="14"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="17">
         <f>COUNTIF(D17:I17,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="18">
+      <c r="A18" s="14">
         <v>4</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="13">
         <f>G15</f>
         <v>0</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="13">
         <f>G16</f>
         <v>0</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="13">
         <f>G17</f>
         <v>0</v>
       </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="21">
+      <c r="G18" s="14"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="17">
         <f>COUNTIF(D18:I18,4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="18">
+      <c r="A19" s="14">
         <v>5</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="13">
         <f>H15</f>
         <v>0</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="13">
         <f>H16</f>
         <v>0</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="13">
         <f>H17</f>
         <v>0</v>
       </c>
-      <c r="G19" s="17">
+      <c r="G19" s="13">
         <f>H18</f>
         <v>0</v>
       </c>
-      <c r="H19" s="18"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="21">
+      <c r="H19" s="14"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="17">
         <f>COUNTIF(D19:I19,5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18">
+      <c r="A20" s="14">
         <v>6</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18" t="s">
+      <c r="B20" s="14"/>
+      <c r="C20" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="13">
         <f>I15</f>
         <v>0</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="13">
         <f>I16</f>
         <v>0</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="13">
         <f>I17</f>
         <v>0</v>
       </c>
-      <c r="G20" s="17">
+      <c r="G20" s="13">
         <f>I18</f>
         <v>0</v>
       </c>
-      <c r="H20" s="17">
+      <c r="H20" s="13">
         <f>I19</f>
         <v>0</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="21">
+      <c r="I20" s="14"/>
+      <c r="J20" s="17">
         <f>COUNTIF(D20:I20,6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="16" t="s">
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="17"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15">
         <v>1</v>
       </c>
-      <c r="E25" s="19">
+      <c r="E25" s="15">
         <v>2</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F25" s="15">
         <v>3</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G25" s="15">
         <v>4</v>
       </c>
-      <c r="H25" s="18"/>
+      <c r="H25" s="14"/>
     </row>
     <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18" t="s">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="18" t="s">
+      <c r="E26" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F26" s="18" t="s">
+      <c r="F26" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G26" s="18" t="s">
+      <c r="G26" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H26" s="18" t="s">
+      <c r="H26" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="18">
+      <c r="A27" s="14">
         <v>1</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="21">
+      <c r="D27" s="14"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="17">
         <f>COUNTIF(D27:G27,1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="18">
+      <c r="A28" s="14">
         <v>2</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="13">
         <f>E27</f>
         <v>0</v>
       </c>
-      <c r="E28" s="18"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="21">
+      <c r="E28" s="14"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="17">
         <f>COUNTIF(D28:G28,2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="18">
+      <c r="A29" s="14">
         <v>3</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="17">
+      <c r="D29" s="13">
         <f>F27</f>
         <v>0</v>
       </c>
-      <c r="E29" s="17">
+      <c r="E29" s="13">
         <f>F28</f>
         <v>0</v>
       </c>
-      <c r="F29" s="18"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="21">
+      <c r="F29" s="14"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="17">
         <f>COUNTIF(D29:G29,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="18">
+      <c r="A30" s="14">
         <v>4</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18" t="s">
+      <c r="B30" s="14"/>
+      <c r="C30" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="17">
+      <c r="D30" s="13">
         <f>G27</f>
         <v>0</v>
       </c>
-      <c r="E30" s="17">
+      <c r="E30" s="13">
         <f>G28</f>
         <v>0</v>
       </c>
-      <c r="F30" s="17">
+      <c r="F30" s="13">
         <f>G29</f>
         <v>0</v>
       </c>
-      <c r="G30" s="18"/>
-      <c r="H30" s="21">
+      <c r="G30" s="14"/>
+      <c r="H30" s="17">
         <f>COUNTIF(D30:G30,4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="16"/>
-      <c r="M35" s="16"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
       <c r="N35" s="12"/>
       <c r="O35" s="11"/>
     </row>
@@ -1823,7 +1823,7 @@
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
-      <c r="N38" s="21">
+      <c r="N38" s="17">
         <f>COUNTIF(D38:M38,1)</f>
         <v>0</v>
       </c>
@@ -1838,7 +1838,7 @@
       <c r="C39" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D39" s="17">
+      <c r="D39" s="13">
         <f>E38</f>
         <v>0</v>
       </c>
@@ -1851,7 +1851,7 @@
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
-      <c r="N39" s="21">
+      <c r="N39" s="17">
         <f>COUNTIF(D39:M39,2)</f>
         <v>0</v>
       </c>
@@ -1866,11 +1866,11 @@
       <c r="C40" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="17">
+      <c r="D40" s="13">
         <f>F38</f>
         <v>0</v>
       </c>
-      <c r="E40" s="17">
+      <c r="E40" s="13">
         <f>F39</f>
         <v>0</v>
       </c>
@@ -1882,7 +1882,7 @@
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
-      <c r="N40" s="21">
+      <c r="N40" s="17">
         <f>COUNTIF(D40:M40,3)</f>
         <v>0</v>
       </c>
@@ -1897,15 +1897,15 @@
       <c r="C41" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D41" s="17">
+      <c r="D41" s="13">
         <f>G38</f>
         <v>0</v>
       </c>
-      <c r="E41" s="17">
+      <c r="E41" s="13">
         <f>G39</f>
         <v>0</v>
       </c>
-      <c r="F41" s="17">
+      <c r="F41" s="13">
         <f>G40</f>
         <v>0</v>
       </c>
@@ -1916,7 +1916,7 @@
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
-      <c r="N41" s="21">
+      <c r="N41" s="17">
         <f>COUNTIF(D41:M41,4)</f>
         <v>0</v>
       </c>
@@ -1931,19 +1931,19 @@
       <c r="C42" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D42" s="17">
+      <c r="D42" s="13">
         <f>H38</f>
         <v>0</v>
       </c>
-      <c r="E42" s="17">
+      <c r="E42" s="13">
         <f>H39</f>
         <v>0</v>
       </c>
-      <c r="F42" s="17">
+      <c r="F42" s="13">
         <f>H40</f>
         <v>0</v>
       </c>
-      <c r="G42" s="17">
+      <c r="G42" s="13">
         <f>H41</f>
         <v>0</v>
       </c>
@@ -1953,7 +1953,7 @@
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
-      <c r="N42" s="21">
+      <c r="N42" s="17">
         <f>COUNTIF(D42:M42,5)</f>
         <v>0</v>
       </c>
@@ -1968,23 +1968,23 @@
       <c r="C43" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D43" s="17">
+      <c r="D43" s="13">
         <f>I38</f>
         <v>0</v>
       </c>
-      <c r="E43" s="17">
+      <c r="E43" s="13">
         <f>I39</f>
         <v>0</v>
       </c>
-      <c r="F43" s="17">
+      <c r="F43" s="13">
         <f>I40</f>
         <v>0</v>
       </c>
-      <c r="G43" s="17">
+      <c r="G43" s="13">
         <f>I41</f>
         <v>0</v>
       </c>
-      <c r="H43" s="17">
+      <c r="H43" s="13">
         <f>I42</f>
         <v>0</v>
       </c>
@@ -1993,7 +1993,7 @@
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
-      <c r="N43" s="21">
+      <c r="N43" s="17">
         <f>COUNTIF(D43:M43,6)</f>
         <v>0</v>
       </c>
@@ -2008,27 +2008,27 @@
       <c r="C44" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D44" s="17">
+      <c r="D44" s="13">
         <f>J38</f>
         <v>0</v>
       </c>
-      <c r="E44" s="17">
+      <c r="E44" s="13">
         <f>J39</f>
         <v>0</v>
       </c>
-      <c r="F44" s="17">
+      <c r="F44" s="13">
         <f>J40</f>
         <v>0</v>
       </c>
-      <c r="G44" s="17">
+      <c r="G44" s="13">
         <f>J41</f>
         <v>0</v>
       </c>
-      <c r="H44" s="17">
+      <c r="H44" s="13">
         <f>J42</f>
         <v>0</v>
       </c>
-      <c r="I44" s="17">
+      <c r="I44" s="13">
         <f>J43</f>
         <v>0</v>
       </c>
@@ -2036,7 +2036,7 @@
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
-      <c r="N44" s="21">
+      <c r="N44" s="17">
         <f>COUNTIF(D44:M44,7)</f>
         <v>0</v>
       </c>
@@ -2051,38 +2051,38 @@
       <c r="C45" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D45" s="17">
+      <c r="D45" s="13">
         <f>K38</f>
         <v>0</v>
       </c>
-      <c r="E45" s="17">
+      <c r="E45" s="13">
         <f>K39</f>
         <v>0</v>
       </c>
-      <c r="F45" s="17">
+      <c r="F45" s="13">
         <f>K40</f>
         <v>0</v>
       </c>
-      <c r="G45" s="17">
+      <c r="G45" s="13">
         <f>K41</f>
         <v>0</v>
       </c>
-      <c r="H45" s="17">
+      <c r="H45" s="13">
         <f>K42</f>
         <v>0</v>
       </c>
-      <c r="I45" s="17">
+      <c r="I45" s="13">
         <f>K43</f>
         <v>0</v>
       </c>
-      <c r="J45" s="17">
+      <c r="J45" s="13">
         <f>K44</f>
         <v>0</v>
       </c>
       <c r="K45" s="2"/>
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
-      <c r="N45" s="21">
+      <c r="N45" s="17">
         <f>COUNTIF(D45:M45,8)</f>
         <v>0</v>
       </c>
@@ -2097,41 +2097,41 @@
       <c r="C46" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D46" s="17">
+      <c r="D46" s="13">
         <f>L38</f>
         <v>0</v>
       </c>
-      <c r="E46" s="17">
+      <c r="E46" s="13">
         <f>L39</f>
         <v>0</v>
       </c>
-      <c r="F46" s="17">
+      <c r="F46" s="13">
         <f>L40</f>
         <v>0</v>
       </c>
-      <c r="G46" s="17">
+      <c r="G46" s="13">
         <f>L41</f>
         <v>0</v>
       </c>
-      <c r="H46" s="17">
+      <c r="H46" s="13">
         <f>L42</f>
         <v>0</v>
       </c>
-      <c r="I46" s="17">
+      <c r="I46" s="13">
         <f>L43</f>
         <v>0</v>
       </c>
-      <c r="J46" s="17">
+      <c r="J46" s="13">
         <f>L44</f>
         <v>0</v>
       </c>
-      <c r="K46" s="17">
+      <c r="K46" s="13">
         <f>L45</f>
         <v>0</v>
       </c>
       <c r="L46" s="2"/>
       <c r="M46" s="4"/>
-      <c r="N46" s="21">
+      <c r="N46" s="17">
         <f>COUNTIF(D46:M46,9)</f>
         <v>0</v>
       </c>
@@ -2146,44 +2146,44 @@
       <c r="C47" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D47" s="17">
+      <c r="D47" s="13">
         <f>M38</f>
         <v>0</v>
       </c>
-      <c r="E47" s="17">
+      <c r="E47" s="13">
         <f>M39</f>
         <v>0</v>
       </c>
-      <c r="F47" s="17">
+      <c r="F47" s="13">
         <f>M40</f>
         <v>0</v>
       </c>
-      <c r="G47" s="17">
+      <c r="G47" s="13">
         <f>M41</f>
         <v>0</v>
       </c>
-      <c r="H47" s="17">
+      <c r="H47" s="13">
         <f>M42</f>
         <v>0</v>
       </c>
-      <c r="I47" s="17">
+      <c r="I47" s="13">
         <f>M43</f>
         <v>0</v>
       </c>
-      <c r="J47" s="17">
+      <c r="J47" s="13">
         <f>M44</f>
         <v>0</v>
       </c>
-      <c r="K47" s="17">
+      <c r="K47" s="13">
         <f>M45</f>
         <v>0</v>
       </c>
-      <c r="L47" s="17">
+      <c r="L47" s="13">
         <f>M46</f>
         <v>0</v>
       </c>
       <c r="M47" s="2"/>
-      <c r="N47" s="21">
+      <c r="N47" s="17">
         <f>COUNTIF(D47:M47,10)</f>
         <v>0</v>
       </c>
@@ -2254,13 +2254,13 @@
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="22"/>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>

</xml_diff>